<commit_message>
Updated the solution for Reverse Words.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jagdish Kamadi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1841D44-C47F-4C62-B68D-DFD478AF075C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0EAC16-07F1-4157-9FD7-02F655FF9567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="207">
   <si>
     <t>Problem</t>
   </si>
@@ -653,6 +653,9 @@
   </si>
   <si>
     <t>Second most repeated string in a sequence</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -994,10 +997,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="44.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1012,6 +1018,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1720,9 +1729,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="36.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1735,6 +1749,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2222,7 +2239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>

<commit_message>
Updated the solution for Parenthesis Checker.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0EAC16-07F1-4157-9FD7-02F655FF9567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D13267-0F6E-48FF-9B93-9F149279F39C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="207">
   <si>
     <t>Problem</t>
   </si>
@@ -997,7 +997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1944,9 +1944,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1964,6 +1970,9 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Middle of a Linked List.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D13267-0F6E-48FF-9B93-9F149279F39C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4465E26-FC8D-4B14-ABE5-11607F0EB409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="207">
   <si>
     <t>Problem</t>
   </si>
@@ -1828,9 +1828,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1843,6 +1849,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1944,7 +1953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the solution for left view of binary tree.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4465E26-FC8D-4B14-ABE5-11607F0EB409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E452A7-A338-4D1E-A071-9A7E64C25523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="207">
   <si>
     <t>Problem</t>
   </si>
@@ -1828,7 +1828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1954,7 +1954,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1975,13 +1975,13 @@
       <c r="A2" t="s">
         <v>56</v>
       </c>
+      <c r="B2" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>57</v>
-      </c>
-      <c r="B3" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2038,9 +2038,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="49.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2053,6 +2059,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2257,9 +2266,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="62.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Updated the solution for Reverse a linked list.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E452A7-A338-4D1E-A071-9A7E64C25523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5431F81-173B-4CBC-B94B-2747B290DD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -18,24 +18,21 @@
     <sheet name="Linked List" sheetId="3" r:id="rId3"/>
     <sheet name="Stack and Queue" sheetId="4" r:id="rId4"/>
     <sheet name="Tree" sheetId="5" r:id="rId5"/>
-    <sheet name="Heap" sheetId="6" r:id="rId6"/>
-    <sheet name="Recursion" sheetId="7" r:id="rId7"/>
-    <sheet name="Hashing" sheetId="8" r:id="rId8"/>
-    <sheet name="Graph" sheetId="9" r:id="rId9"/>
-    <sheet name="Greedy" sheetId="10" r:id="rId10"/>
-    <sheet name="Dynamic Programming" sheetId="11" r:id="rId11"/>
-    <sheet name="Divide and Conquer" sheetId="12" r:id="rId12"/>
-    <sheet name="Backtracking" sheetId="13" r:id="rId13"/>
-    <sheet name="Bit Magic" sheetId="14" r:id="rId14"/>
-    <sheet name="Some More Questions on Arrays" sheetId="15" r:id="rId15"/>
-    <sheet name="Some More Questions on Strings" sheetId="16" r:id="rId16"/>
+    <sheet name="Recursion" sheetId="7" r:id="rId6"/>
+    <sheet name="Hashing" sheetId="8" r:id="rId7"/>
+    <sheet name="Dynamic Programming" sheetId="11" r:id="rId8"/>
+    <sheet name="Divide and Conquer" sheetId="12" r:id="rId9"/>
+    <sheet name="Backtracking" sheetId="13" r:id="rId10"/>
+    <sheet name="Bit Magic" sheetId="14" r:id="rId11"/>
+    <sheet name="Some More Questions on Arrays" sheetId="15" r:id="rId12"/>
+    <sheet name="Some More Questions on Strings" sheetId="16" r:id="rId13"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="173">
   <si>
     <t>Problem</t>
   </si>
@@ -283,24 +280,6 @@
     <t>Serialize and Deserialize a Binary Tree</t>
   </si>
   <si>
-    <t>Find median in a stream</t>
-  </si>
-  <si>
-    <t>Heap Sort</t>
-  </si>
-  <si>
-    <t>Operations on Binary Min Heap</t>
-  </si>
-  <si>
-    <t>Rearrange characters</t>
-  </si>
-  <si>
-    <t>Merge K sorted linked lists</t>
-  </si>
-  <si>
-    <t>Kth largest element in a stream</t>
-  </si>
-  <si>
     <t>Flood fill Algorithm</t>
   </si>
   <si>
@@ -371,90 +350,6 @@
   </si>
   <si>
     <t>Check if frequencies can be equal</t>
-  </si>
-  <si>
-    <t>Depth First Traversal</t>
-  </si>
-  <si>
-    <t>Breadth First Traversal</t>
-  </si>
-  <si>
-    <t>Detect cycle in undirected graph</t>
-  </si>
-  <si>
-    <t>Detect cycle in a directed graph</t>
-  </si>
-  <si>
-    <t>Topological sort</t>
-  </si>
-  <si>
-    <t>Find the number of islands</t>
-  </si>
-  <si>
-    <t>Implementing Dijkstra</t>
-  </si>
-  <si>
-    <t>Minimum Swaps</t>
-  </si>
-  <si>
-    <t>Strongly Connected Components</t>
-  </si>
-  <si>
-    <t>Shortest Source to Destination Path</t>
-  </si>
-  <si>
-    <t>Find whether path exist</t>
-  </si>
-  <si>
-    <t>Minimum Cost Path</t>
-  </si>
-  <si>
-    <t>Circle of Strings</t>
-  </si>
-  <si>
-    <t>Floyd Warshall</t>
-  </si>
-  <si>
-    <t>Alien Dictionary</t>
-  </si>
-  <si>
-    <t>Snake and Ladder Problem</t>
-  </si>
-  <si>
-    <t>Activity Selection</t>
-  </si>
-  <si>
-    <t>N meetings in one room</t>
-  </si>
-  <si>
-    <t>Coin Piles</t>
-  </si>
-  <si>
-    <t>Maximize Toys</t>
-  </si>
-  <si>
-    <t>Page Faults in LRU</t>
-  </si>
-  <si>
-    <t>Largest number possible</t>
-  </si>
-  <si>
-    <t>Minimize the heights</t>
-  </si>
-  <si>
-    <t>Minimize the sum of product</t>
-  </si>
-  <si>
-    <t>Huffman Decoding</t>
-  </si>
-  <si>
-    <t>Minimum Spanning Tree</t>
-  </si>
-  <si>
-    <t>Shop in Candy Store</t>
-  </si>
-  <si>
-    <t>Geek collects the balls</t>
   </si>
   <si>
     <t>Minimum Operations</t>
@@ -1020,7 +915,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1144,279 +1039,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13" xr:uid="{00000000-0002-0000-0900-000000000000}">
-      <formula1>"Done,Not Done"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>159</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15 B16 B17 B18 B19 B20 B21" xr:uid="{00000000-0002-0000-0A00-000000000000}">
-      <formula1>"Done,Not Done"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8" xr:uid="{00000000-0002-0000-0B00-000000000000}">
-      <formula1>"Done,Not Done"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1434,27 +1056,27 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1467,7 +1089,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -1485,72 +1107,72 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1563,11 +1185,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1581,47 +1205,47 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>194</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1634,7 +1258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -1652,27 +1276,27 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1682,37 +1306,37 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>204</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>205</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1751,7 +1375,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1829,7 +1453,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1851,12 +1475,15 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1976,7 +1603,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2038,8 +1665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2061,7 +1688,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2150,64 +1777,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7" xr:uid="{00000000-0002-0000-0500-000000000000}">
-      <formula1>"Done,Not Done"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2229,27 +1798,27 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2262,7 +1831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -2286,97 +1855,97 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2389,9 +1958,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:B17"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2407,87 +1976,168 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15 B16 B17" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15 B16 B17 B18 B19 B20 B21" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+      <formula1>"Done,Not Done"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>"Done,Not Done"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated the solution for Missing And Repeating.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5431F81-173B-4CBC-B94B-2747B290DD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A719707-3A37-4DE1-93F0-E3DE0D34654C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="173">
   <si>
     <t>Problem</t>
   </si>
@@ -1190,10 +1190,14 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1206,6 +1210,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Sort according to an Array.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,31 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A719707-3A37-4DE1-93F0-E3DE0D34654C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C356637-544A-4DAC-B7DD-0B8A403BEE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
     <sheet name="String" sheetId="2" r:id="rId2"/>
     <sheet name="Linked List" sheetId="3" r:id="rId3"/>
     <sheet name="Stack and Queue" sheetId="4" r:id="rId4"/>
-    <sheet name="Tree" sheetId="5" r:id="rId5"/>
-    <sheet name="Recursion" sheetId="7" r:id="rId6"/>
-    <sheet name="Hashing" sheetId="8" r:id="rId7"/>
-    <sheet name="Dynamic Programming" sheetId="11" r:id="rId8"/>
-    <sheet name="Divide and Conquer" sheetId="12" r:id="rId9"/>
-    <sheet name="Backtracking" sheetId="13" r:id="rId10"/>
-    <sheet name="Bit Magic" sheetId="14" r:id="rId11"/>
-    <sheet name="Some More Questions on Arrays" sheetId="15" r:id="rId12"/>
-    <sheet name="Some More Questions on Strings" sheetId="16" r:id="rId13"/>
+    <sheet name="Hashing" sheetId="8" r:id="rId5"/>
+    <sheet name="Dynamic Programming" sheetId="11" r:id="rId6"/>
+    <sheet name="Divide and Conquer" sheetId="12" r:id="rId7"/>
+    <sheet name="Backtracking" sheetId="13" r:id="rId8"/>
+    <sheet name="Bit Magic" sheetId="14" r:id="rId9"/>
+    <sheet name="Some More Questions on Arrays" sheetId="15" r:id="rId10"/>
+    <sheet name="Some More Questions on Strings" sheetId="16" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="152">
   <si>
     <t>Problem</t>
   </si>
@@ -230,69 +228,6 @@
   </si>
   <si>
     <t>Maximum of all subarrays of size k</t>
-  </si>
-  <si>
-    <t>Print Left View of Binary Tree</t>
-  </si>
-  <si>
-    <t>Check for BST</t>
-  </si>
-  <si>
-    <t>Print Bottom View of Binary Tree</t>
-  </si>
-  <si>
-    <t>Print a Binary Tree in Vertical Order</t>
-  </si>
-  <si>
-    <t>Level order traversal in spiral form</t>
-  </si>
-  <si>
-    <t>Connect Nodes at Same Level</t>
-  </si>
-  <si>
-    <t>Lowest Common Ancestor in a BST</t>
-  </si>
-  <si>
-    <t>Convert a given Binary Tree to Doubly Linked List</t>
-  </si>
-  <si>
-    <t>Write Code to Determine if Two Trees are Identical or Not</t>
-  </si>
-  <si>
-    <t>Given a binary tree, check whether it is a mirror of itself</t>
-  </si>
-  <si>
-    <t>Height of Binary Tree</t>
-  </si>
-  <si>
-    <t>Maximum Path Sum</t>
-  </si>
-  <si>
-    <t>Diameter of a Binary Tree</t>
-  </si>
-  <si>
-    <t>Number of leaf nodes</t>
-  </si>
-  <si>
-    <t>Check if given Binary Tree is Height Balanced or Not</t>
-  </si>
-  <si>
-    <t>Serialize and Deserialize a Binary Tree</t>
-  </si>
-  <si>
-    <t>Flood fill Algorithm</t>
-  </si>
-  <si>
-    <t>Number of paths</t>
-  </si>
-  <si>
-    <t>Combination Sum - Part 2</t>
-  </si>
-  <si>
-    <t>Special Keyboard</t>
-  </si>
-  <si>
-    <t>Josephus problem</t>
   </si>
   <si>
     <t>Relative Sorting</t>
@@ -915,7 +850,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1039,157 +974,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6" xr:uid="{00000000-0002-0000-0C00-000000000000}">
-      <formula1>"Done,Not Done"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>151</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15" xr:uid="{00000000-0002-0000-0D00-000000000000}">
-      <formula1>"Done,Not Done"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1209,50 +997,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1265,7 +1053,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -1283,27 +1071,27 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1313,37 +1101,37 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1382,7 +1170,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1482,7 +1270,7 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1490,7 +1278,7 @@
         <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1610,7 +1398,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1669,181 +1457,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="49.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15 B16 B17" xr:uid="{00000000-0002-0000-0400-000000000000}">
-      <formula1>"Done,Not Done"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6" xr:uid="{00000000-0002-0000-0600-000000000000}">
-      <formula1>"Done,Not Done"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1862,97 +1480,100 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1965,7 +1586,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -1983,102 +1604,102 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2091,7 +1712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -2109,37 +1730,37 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2150,4 +1771,151 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+      <formula1>"Done,Not Done"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15" xr:uid="{00000000-0002-0000-0D00-000000000000}">
+      <formula1>"Done,Not Done"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the solution for Activity Selection problem.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C356637-544A-4DAC-B7DD-0B8A403BEE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649BED02-D603-4EC3-9F2A-AF8F7F88ABB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -18,19 +18,20 @@
     <sheet name="Linked List" sheetId="3" r:id="rId3"/>
     <sheet name="Stack and Queue" sheetId="4" r:id="rId4"/>
     <sheet name="Hashing" sheetId="8" r:id="rId5"/>
-    <sheet name="Dynamic Programming" sheetId="11" r:id="rId6"/>
-    <sheet name="Divide and Conquer" sheetId="12" r:id="rId7"/>
-    <sheet name="Backtracking" sheetId="13" r:id="rId8"/>
-    <sheet name="Bit Magic" sheetId="14" r:id="rId9"/>
-    <sheet name="Some More Questions on Arrays" sheetId="15" r:id="rId10"/>
-    <sheet name="Some More Questions on Strings" sheetId="16" r:id="rId11"/>
+    <sheet name="Greedy" sheetId="17" r:id="rId6"/>
+    <sheet name="Dynamic Programming" sheetId="11" r:id="rId7"/>
+    <sheet name="Divide and Conquer" sheetId="12" r:id="rId8"/>
+    <sheet name="Backtracking" sheetId="13" r:id="rId9"/>
+    <sheet name="Bit Magic" sheetId="14" r:id="rId10"/>
+    <sheet name="Some More Questions on Arrays" sheetId="15" r:id="rId11"/>
+    <sheet name="Some More Questions on Strings" sheetId="16" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="164">
   <si>
     <t>Problem</t>
   </si>
@@ -486,6 +487,42 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>1. Activity Selection</t>
+  </si>
+  <si>
+    <t>2. N meetings in one room</t>
+  </si>
+  <si>
+    <t>3. Coin Piles</t>
+  </si>
+  <si>
+    <t>4. Maximize Toys</t>
+  </si>
+  <si>
+    <t>5. Page Faults in LRU</t>
+  </si>
+  <si>
+    <t>6. Largest number possible</t>
+  </si>
+  <si>
+    <t>7. Minimize the heights</t>
+  </si>
+  <si>
+    <t>8. Minimize the sum of product</t>
+  </si>
+  <si>
+    <t>9. Huffman Decoding</t>
+  </si>
+  <si>
+    <t>10. Minimum Spanning Tree</t>
+  </si>
+  <si>
+    <t>11. Shop in Candy Store</t>
+  </si>
+  <si>
+    <t>12. Geek collects the balls</t>
   </si>
 </sst>
 </file>
@@ -974,6 +1011,102 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15" xr:uid="{00000000-0002-0000-0D00-000000000000}">
+      <formula1>"Done,Not Done"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -1053,7 +1186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -1460,8 +1593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1587,12 +1720,122 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911C6CA0-355F-424E-AEDC-886F8054E647}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.geeksforgeeks.org/problems/activity-selection-1587115620/1" xr:uid="{89842E24-2655-4B92-8870-2BDD7F88B7A0}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://www.geeksforgeeks.org/problems/n-meetings-in-one-room-1587115620/1" xr:uid="{E85ED0E8-D5C4-4A67-9855-F4E76DB09134}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://www.geeksforgeeks.org/problems/choose-and-swap0531/1" xr:uid="{F848EB6C-1EB7-49C6-900F-9272B0422084}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://www.geeksforgeeks.org/problems/maximize-toys0331/1" xr:uid="{5A2194C8-A517-4FE9-AA07-FAB126DF6AF2}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://www.geeksforgeeks.org/problems/page-faults-in-lru5603/1" xr:uid="{3AC67436-AE90-4FEE-8673-4B4A2BBB7BB8}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://www.geeksforgeeks.org/problems/largest-number-possible5028/1" xr:uid="{3AE4DC8A-A9D7-4CAC-9046-3BA161A612B3}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://www.geeksforgeeks.org/problems/minimize-the-heights3351/1" xr:uid="{CC06DE0B-CDAB-4614-B6E6-4AAC522475B2}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://www.geeksforgeeks.org/problems/minimize-the-sum-of-product1525/1" xr:uid="{7ED61B9D-AA8B-4790-B984-B0C38C3F35A3}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://www.geeksforgeeks.org/problems/huffman-decoding-1/1" xr:uid="{27B230B6-4F10-48D9-909B-85DD489EE435}"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://www.geeksforgeeks.org/problems/minimum-spanning-tree/1" xr:uid="{F29C9886-6B72-46F6-AA5C-110EEC1739B3}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://www.geeksforgeeks.org/problems/shop-in-candy-store1145/1" xr:uid="{F3143FE4-0620-46D8-967F-9C1D11529F4B}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://www.geeksforgeeks.org/problems/geek-collects-the-balls5515/1" xr:uid="{ECD46EB1-0204-433F-8206-BBD95C2B3DCC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1712,7 +1955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1773,7 +2016,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1822,100 +2065,4 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15" xr:uid="{00000000-0002-0000-0D00-000000000000}">
-      <formula1>"Done,Not Done"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the solution for Search in Rotated Sorted Array.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649BED02-D603-4EC3-9F2A-AF8F7F88ABB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE63C7E-F760-4D13-86EF-AFE1230461C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Stack and Queue" sheetId="4" r:id="rId4"/>
     <sheet name="Hashing" sheetId="8" r:id="rId5"/>
     <sheet name="Greedy" sheetId="17" r:id="rId6"/>
-    <sheet name="Dynamic Programming" sheetId="11" r:id="rId7"/>
+    <sheet name="Dynamic Programming" sheetId="18" r:id="rId7"/>
     <sheet name="Divide and Conquer" sheetId="12" r:id="rId8"/>
     <sheet name="Backtracking" sheetId="13" r:id="rId9"/>
     <sheet name="Bit Magic" sheetId="14" r:id="rId10"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="164">
   <si>
     <t>Problem</t>
   </si>
@@ -288,66 +288,6 @@
     <t>Check if frequencies can be equal</t>
   </si>
   <si>
-    <t>Minimum Operations</t>
-  </si>
-  <si>
-    <t>Max length chain</t>
-  </si>
-  <si>
-    <t>Minimum number of Coins</t>
-  </si>
-  <si>
-    <t>Longest Common Substring</t>
-  </si>
-  <si>
-    <t>Longest Increasing Subsequence</t>
-  </si>
-  <si>
-    <t>Longest Common Subsequence</t>
-  </si>
-  <si>
-    <t>0 - 1 Knapsack Problem</t>
-  </si>
-  <si>
-    <t>Maximum sum increasing subsequence</t>
-  </si>
-  <si>
-    <t>Minimum number of jumps</t>
-  </si>
-  <si>
-    <t>Edit Distance</t>
-  </si>
-  <si>
-    <t>Coin Change Problem</t>
-  </si>
-  <si>
-    <t>Subset Sum Problem</t>
-  </si>
-  <si>
-    <t>Box Stacking</t>
-  </si>
-  <si>
-    <t>Rod Cutting</t>
-  </si>
-  <si>
-    <t>Path in Matrix</t>
-  </si>
-  <si>
-    <t>Minimum sum partition</t>
-  </si>
-  <si>
-    <t>Count number of ways to cover a distance</t>
-  </si>
-  <si>
-    <t>Egg Dropping Puzzle</t>
-  </si>
-  <si>
-    <t>Optimal Strategy for a Game</t>
-  </si>
-  <si>
-    <t>Shortest Common Supersequence</t>
-  </si>
-  <si>
     <t>Find the element that appears once in sorted array</t>
   </si>
   <si>
@@ -523,6 +463,66 @@
   </si>
   <si>
     <t>12. Geek collects the balls</t>
+  </si>
+  <si>
+    <t>1. Minimum Operations</t>
+  </si>
+  <si>
+    <t>2. Max length chain</t>
+  </si>
+  <si>
+    <t>3. Minimum number of Coins</t>
+  </si>
+  <si>
+    <t>4. Longest Common Substring</t>
+  </si>
+  <si>
+    <t>5. Longest Increasing Subsequence</t>
+  </si>
+  <si>
+    <t>6. Longest Common Subsequence</t>
+  </si>
+  <si>
+    <t>7. 0 - 1 Knapsack Problem</t>
+  </si>
+  <si>
+    <t>8. Maximum sum increasing subsequence</t>
+  </si>
+  <si>
+    <t>9. Minimum number of jumps</t>
+  </si>
+  <si>
+    <t>10. Edit Distance</t>
+  </si>
+  <si>
+    <t>11. Coin Change Problem</t>
+  </si>
+  <si>
+    <t>12. Subset Sum Problem</t>
+  </si>
+  <si>
+    <t>13. Box Stacking</t>
+  </si>
+  <si>
+    <t>14. Rod Cutting</t>
+  </si>
+  <si>
+    <t>15. Path in Matrix</t>
+  </si>
+  <si>
+    <t>16. Minimum sum partition</t>
+  </si>
+  <si>
+    <t>17. Count number of ways to cover a distance</t>
+  </si>
+  <si>
+    <t>18. Egg Dropping Puzzle</t>
+  </si>
+  <si>
+    <t>19. Optimal Strategy for a Game</t>
+  </si>
+  <si>
+    <t>20. Shortest Common Supersequence</t>
   </si>
 </sst>
 </file>
@@ -887,7 +887,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1028,72 +1028,72 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1130,50 +1130,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
         <v>131</v>
-      </c>
-      <c r="B2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1204,17 +1204,17 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1224,7 +1224,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1234,37 +1234,37 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1303,7 +1303,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1403,7 +1403,7 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1411,7 +1411,7 @@
         <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1531,7 +1531,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1616,7 +1616,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1723,14 +1723,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911C6CA0-355F-424E-AEDC-886F8054E647}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1743,68 +1743,76 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6" xr:uid="{A0AE3C08-0B42-402C-99A5-E80BDAE8E853}">
+      <formula1>"Done,Not Done"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://www.geeksforgeeks.org/problems/activity-selection-1587115620/1" xr:uid="{89842E24-2655-4B92-8870-2BDD7F88B7A0}"/>
     <hyperlink ref="A3" r:id="rId2" display="https://www.geeksforgeeks.org/problems/n-meetings-in-one-room-1587115620/1" xr:uid="{E85ED0E8-D5C4-4A67-9855-F4E76DB09134}"/>
@@ -1824,16 +1832,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA610411-C414-4A98-9C12-411E178D324C}">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1847,111 +1855,128 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15 B16 B17 B18 B19 B20 B21" xr:uid="{00000000-0002-0000-0A00-000000000000}">
-      <formula1>"Done,Not Done"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.geeksforgeeks.org/problems/find-optimum-operation4504/1" xr:uid="{2E3E9654-CB1B-4769-AED8-2DA411C8765C}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://www.geeksforgeeks.org/dsa/maximum-length-chain-of-pairs-dp-20/" xr:uid="{C7671AAA-93C7-41BE-B89B-AC0BAB710F1E}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://www.geeksforgeeks.org/problems/-minimum-number-of-coins4426/1" xr:uid="{78D9910D-A990-4B38-915A-5E1B63CC4014}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://www.geeksforgeeks.org/problems/longest-common-substring1452/1" xr:uid="{49E7EB5B-B94A-4DF7-BF8C-FB2023913BCF}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://www.geeksforgeeks.org/problems/longest-increasing-subsequence-1587115620/1" xr:uid="{79A1BB66-78D9-499C-B9F8-F10D9AAB9AEE}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://www.geeksforgeeks.org/problems/longest-common-subsequence-1587115620/1" xr:uid="{F63B32D5-D18D-478A-8661-757D2DF6C2BB}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://www.geeksforgeeks.org/problems/0-1-knapsack-problem0945/1" xr:uid="{3FA7685B-945A-47C9-A6F7-92BE240AFAA6}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://www.geeksforgeeks.org/problems/maximum-sum-increasing-subsequence4749/1" xr:uid="{40E5BC6B-7027-44E2-9F95-9531D116A1BB}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://www.geeksforgeeks.org/problems/minimum-number-of-jumps-1587115620/1" xr:uid="{E2AF0468-319D-4EEA-9C19-730DCD71EF48}"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://www.geeksforgeeks.org/problems/edit-distance3702/1" xr:uid="{C1D2C48E-8E7F-4B7A-9B34-023F0F1B5630}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://www.geeksforgeeks.org/problems/coin-change2448/1" xr:uid="{31B735D7-7732-4788-A165-154D0AF62461}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://www.geeksforgeeks.org/problems/subset-sum-problem2014/1" xr:uid="{81928F6B-A1EB-409D-9CD0-62BC96851B8C}"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://www.geeksforgeeks.org/problems/box-stacking/1" xr:uid="{0BF4628A-67B4-44F8-AAAA-B242EDEF7819}"/>
+    <hyperlink ref="A15" r:id="rId14" display="https://www.geeksforgeeks.org/problems/cutted-segments1642/1" xr:uid="{8644DF88-4678-428F-8C1C-7D693CE184D9}"/>
+    <hyperlink ref="A16" r:id="rId15" display="https://www.geeksforgeeks.org/dsa/find-the-longest-path-in-a-matrix-with-given-constraints/" xr:uid="{6269DF6F-ACDC-4EC9-8320-713926AF88FB}"/>
+    <hyperlink ref="A17" r:id="rId16" display="https://www.geeksforgeeks.org/problems/minimum-sum-partition3317/1" xr:uid="{72F45689-424D-4089-A095-A9B5C20A0381}"/>
+    <hyperlink ref="A18" r:id="rId17" display="https://www.geeksforgeeks.org/problems/count-number-of-hops-1587115620/1" xr:uid="{B9495097-B294-4970-BCC7-DEBE44346512}"/>
+    <hyperlink ref="A19" r:id="rId18" display="https://www.geeksforgeeks.org/problems/egg-dropping-puzzle-1587115620/1" xr:uid="{17E925D0-7C97-40D4-B129-03B5BE982C97}"/>
+    <hyperlink ref="A20" r:id="rId19" display="https://www.geeksforgeeks.org/problems/optimal-strategy-for-a-game-1587115620/1" xr:uid="{AE596B73-36A8-49C7-B1C6-485EC6F73230}"/>
+    <hyperlink ref="A21" r:id="rId20" display="https://www.geeksforgeeks.org/problems/shortest-common-supersequence0322/1" xr:uid="{56F3FFAE-AEBE-4DD0-A5B3-8602718F2479}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1959,9 +1984,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="43.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1973,37 +2004,43 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2020,9 +2057,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2034,27 +2077,27 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the solution for Permutations of a String problem.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE63C7E-F760-4D13-86EF-AFE1230461C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300CD802-1505-4B8F-ADD6-E410F7BB2E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="164">
   <si>
     <t>Problem</t>
   </si>
@@ -1281,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1309,6 +1309,9 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1984,7 +1987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the solution for Minimum Operations problem.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300CD802-1505-4B8F-ADD6-E410F7BB2E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECCB6B1-1FD9-44ED-BC2D-841D087BFBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,15 @@
     <sheet name="Greedy" sheetId="17" r:id="rId6"/>
     <sheet name="Dynamic Programming" sheetId="18" r:id="rId7"/>
     <sheet name="Divide and Conquer" sheetId="12" r:id="rId8"/>
-    <sheet name="Backtracking" sheetId="13" r:id="rId9"/>
-    <sheet name="Bit Magic" sheetId="14" r:id="rId10"/>
-    <sheet name="Some More Questions on Arrays" sheetId="15" r:id="rId11"/>
-    <sheet name="Some More Questions on Strings" sheetId="16" r:id="rId12"/>
+    <sheet name="Some More Questions on Arrays" sheetId="15" r:id="rId9"/>
+    <sheet name="Some More Questions on Strings" sheetId="16" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="145">
   <si>
     <t>Problem</t>
   </si>
@@ -307,63 +305,6 @@
   </si>
   <si>
     <t>K-th element of two sorted Arrays</t>
-  </si>
-  <si>
-    <t>N-Queen Problem</t>
-  </si>
-  <si>
-    <t>Solve the Sudoku</t>
-  </si>
-  <si>
-    <t>Rat in a Maze Problem</t>
-  </si>
-  <si>
-    <t>Word Boggle</t>
-  </si>
-  <si>
-    <t>Generate IP Addresses</t>
-  </si>
-  <si>
-    <t>Find first set bit</t>
-  </si>
-  <si>
-    <t>Rightmost different bit</t>
-  </si>
-  <si>
-    <t>Check whether K-th bit is set or not</t>
-  </si>
-  <si>
-    <t>Toggle bits given range</t>
-  </si>
-  <si>
-    <t>Set kth bit</t>
-  </si>
-  <si>
-    <t>Power of 2</t>
-  </si>
-  <si>
-    <t>Bit Difference</t>
-  </si>
-  <si>
-    <t>Rotate Bits</t>
-  </si>
-  <si>
-    <t>Swap all odd and even bits</t>
-  </si>
-  <si>
-    <t>Count total set bits</t>
-  </si>
-  <si>
-    <t>Longest Consecutive 1's</t>
-  </si>
-  <si>
-    <t>Sparse Number</t>
-  </si>
-  <si>
-    <t>Alone in a couple</t>
-  </si>
-  <si>
-    <t>Maximum subset XOR</t>
   </si>
   <si>
     <t>Find Missing And Repeating</t>
@@ -887,7 +828,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1011,112 +952,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10 B11 B12 B13 B14 B15" xr:uid="{00000000-0002-0000-0D00-000000000000}">
-      <formula1>"Done,Not Done"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1130,91 +975,20 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10" xr:uid="{00000000-0002-0000-0E00-000000000000}">
-      <formula1>"Done,Not Done"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:B14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1224,7 +998,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1234,37 +1008,37 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1281,7 +1055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1303,7 +1077,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1311,7 +1085,7 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1406,7 +1180,7 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1414,7 +1188,7 @@
         <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1534,7 +1308,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1619,7 +1393,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1746,68 +1520,68 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1838,8 +1612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA610411-C414-4A98-9C12-411E178D324C}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1858,105 +1632,116 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>126</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8" xr:uid="{3BBC69B5-5BF8-4B95-800D-F12009AD2024}">
+      <formula1>"Done,Not Done"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://www.geeksforgeeks.org/problems/find-optimum-operation4504/1" xr:uid="{2E3E9654-CB1B-4769-AED8-2DA411C8765C}"/>
     <hyperlink ref="A3" r:id="rId2" display="https://www.geeksforgeeks.org/dsa/maximum-length-chain-of-pairs-dp-20/" xr:uid="{C7671AAA-93C7-41BE-B89B-AC0BAB710F1E}"/>
@@ -1988,7 +1773,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2010,7 +1795,7 @@
         <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2018,7 +1803,7 @@
         <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2057,16 +1842,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2082,6 +1867,9 @@
       <c r="A2" t="s">
         <v>92</v>
       </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -2103,9 +1891,29 @@
         <v>96</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B3 B4 B5 B6 B7 B8 B9 B10" xr:uid="{00000000-0002-0000-0E00-000000000000}">
       <formula1>"Done,Not Done"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated the solution for Next Greater Element problem.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECCB6B1-1FD9-44ED-BC2D-841D087BFBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB352B09-0A91-49D1-A49D-1EC65878D99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="145">
   <si>
     <t>Problem</t>
   </si>
@@ -806,7 +806,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -834,6 +834,9 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1285,8 +1288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1314,6 +1317,9 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1612,7 +1618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA610411-C414-4A98-9C12-411E178D324C}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the solution for Sorting Elements of an Array by Frequency problem.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB352B09-0A91-49D1-A49D-1EC65878D99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161C831D-F151-432B-92DD-FADE0439C27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="145">
   <si>
     <t>Problem</t>
   </si>
@@ -1288,7 +1288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1376,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1405,6 +1405,9 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Rotate a Linked List problem.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161C831D-F151-432B-92DD-FADE0439C27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E655F109-EAA9-4E53-9073-E0E4E96CEF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="146">
   <si>
     <t>Problem</t>
   </si>
@@ -464,6 +464,9 @@
   </si>
   <si>
     <t>20. Shortest Common Supersequence</t>
+  </si>
+  <si>
+    <t>Not Done</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1197,6 +1200,9 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1376,7 +1382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1855,7 +1861,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1884,6 +1890,9 @@
       <c r="A3" t="s">
         <v>93</v>
       </c>
+      <c r="B3" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
Updated the solution for Kadane's Algorithm problem.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E655F109-EAA9-4E53-9073-E0E4E96CEF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1169F855-54F9-4A94-8054-2969D731B48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="146">
   <si>
     <t>Problem</t>
   </si>
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -845,6 +845,9 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1163,7 +1166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the solution for Largest subarray with 0 sum problem.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1169F855-54F9-4A94-8054-2969D731B48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFDC6A3-E35F-44C1-9D99-F41D1FF93AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="146">
   <si>
     <t>Problem</t>
   </si>
@@ -808,7 +808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1385,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1422,6 +1422,9 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Stack using two queues and Queue using two Stacks problems.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFDC6A3-E35F-44C1-9D99-F41D1FF93AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F239F8D8-CE7D-460D-85C0-DBCE67E62238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="146">
   <si>
     <t>Problem</t>
   </si>
@@ -1297,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1335,10 +1335,16 @@
       <c r="A4" t="s">
         <v>58</v>
       </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -1385,7 +1391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the solution for Minimum number of Coins problem.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F239F8D8-CE7D-460D-85C0-DBCE67E62238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE881309-C903-415F-B0B2-E23A389B477D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="146">
   <si>
     <t>Problem</t>
   </si>
@@ -1297,7 +1297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1528,7 +1528,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1564,6 +1564,9 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1639,8 +1642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA610411-C414-4A98-9C12-411E178D324C}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1676,6 +1679,9 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>127</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated the solution for Sum of Middle elements of two sorted arrays problem.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE881309-C903-415F-B0B2-E23A389B477D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22586561-20FE-452A-AD90-3F6854F35908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="148">
   <si>
     <t>Problem</t>
   </si>
@@ -467,6 +467,12 @@
   </si>
   <si>
     <t>Not Done</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Problem is not available</t>
   </si>
 </sst>
 </file>
@@ -1642,7 +1648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA610411-C414-4A98-9C12-411E178D324C}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1803,27 +1809,31 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="43.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -1831,7 +1841,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -1839,27 +1849,36 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
Updated the code for Consecutive 1's not allowed problem.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22586561-20FE-452A-AD90-3F6854F35908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F03A0F-A45A-46E1-A9F5-252B30B4981E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="148">
   <si>
     <t>Problem</t>
   </si>
@@ -1811,7 +1811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1897,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1935,6 +1935,9 @@
       <c r="A4" t="s">
         <v>94</v>
       </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
Updated the solution for CamelCase Pattern Matching problem.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F03A0F-A45A-46E1-A9F5-252B30B4981E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F461EE-F9CC-4B68-A4C9-05C081821506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="148">
   <si>
     <t>Problem</t>
   </si>
@@ -970,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -999,6 +999,9 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1897,7 +1900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the solution for String Ignorance problem.
</commit_message>
<xml_diff>
--- a/Coding_Tracker.xlsx
+++ b/Coding_Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyWork\codevault\gfg-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B54132F-744B-4D37-8C41-6AC9EFC17071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B83D79-EAD1-4A1D-A6C4-170453BFCBA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="148">
   <si>
     <t>Problem</t>
   </si>
@@ -971,7 +971,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1007,6 +1007,9 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>